<commit_message>
Add rubrics for final project
</commit_message>
<xml_diff>
--- a/static/files/blank_dei.xlsx
+++ b/static/files/blank_dei.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/andrew/Dropbox/Teaching/• Courses/Introduction to nonprofits/2022-Spring/Rubrics/05 DEI/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/andrew/Sites/courses/nonprofitsp22/static/files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3274A682-B751-4840-9A94-2D3DAF3E9B97}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8145FC9B-E8B8-7849-8DDE-2222E07A8807}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17720" xr2:uid="{AE642143-4B0F-CF4A-8303-14EA69BAC89B}"/>
+    <workbookView xWindow="4360" yWindow="4460" windowWidth="30240" windowHeight="17720" xr2:uid="{AE642143-4B0F-CF4A-8303-14EA69BAC89B}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -148,13 +148,13 @@
     <t>Implementation</t>
   </si>
   <si>
-    <t>15–11</t>
-  </si>
-  <si>
-    <t>10–6</t>
-  </si>
-  <si>
-    <t>5–0</t>
+    <t>5–4</t>
+  </si>
+  <si>
+    <t>3–2</t>
+  </si>
+  <si>
+    <t>1–0</t>
   </si>
 </sst>
 </file>
@@ -379,7 +379,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="40">
+  <cellXfs count="41">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top"/>
@@ -497,6 +497,9 @@
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -942,16 +945,16 @@
         <v>30</v>
       </c>
       <c r="D11" s="17">
-        <v>10</v>
-      </c>
-      <c r="E11" s="18" t="s">
-        <v>22</v>
+        <v>5</v>
+      </c>
+      <c r="E11" s="40" t="s">
+        <v>36</v>
       </c>
       <c r="F11" s="18" t="s">
-        <v>23</v>
+        <v>37</v>
       </c>
       <c r="G11" s="18" t="s">
-        <v>24</v>
+        <v>38</v>
       </c>
       <c r="H11" s="19"/>
     </row>
@@ -983,7 +986,7 @@
       </c>
       <c r="D13" s="33">
         <f>SUM(D10:D12)</f>
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="E13" s="36">
         <f>IF(calc_stuff="Yes", SUM(E10:G12), 0)</f>
@@ -1027,16 +1030,16 @@
         <v>34</v>
       </c>
       <c r="D17" s="17">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="E17" s="18" t="s">
-        <v>36</v>
+        <v>22</v>
       </c>
       <c r="F17" s="18" t="s">
-        <v>37</v>
+        <v>23</v>
       </c>
       <c r="G17" s="18" t="s">
-        <v>38</v>
+        <v>24</v>
       </c>
       <c r="H17" s="19"/>
     </row>
@@ -1047,7 +1050,7 @@
       </c>
       <c r="D18" s="33">
         <f>SUM(D17:D17)</f>
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="E18" s="36">
         <f>IF(calc_stuff="Yes", SUM(E17:G17), 0)</f>
@@ -1178,7 +1181,7 @@
       </c>
       <c r="D27" s="5">
         <f>D13+D18+D25</f>
-        <v>50</v>
+        <v>40</v>
       </c>
       <c r="E27" s="35">
         <f>IF(calc_stuff="Yes", SUM(E22:G24), 0)</f>

</xml_diff>